<commit_message>
more output, but errors need fixing
</commit_message>
<xml_diff>
--- a/output/preprocessing/ind_timeseries_specific_consumption.xlsx
+++ b/output/preprocessing/ind_timeseries_specific_consumption.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM34"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4729,7 +4729,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -4741,19 +4741,19 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>-5428.807777775573</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>2.735666666666</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>36880335.97316612</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>-37012.58894130614</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>9.286333318611</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -4768,14 +4768,20 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L33" t="n">
-        <v>23.735666666667</v>
-      </c>
-      <c r="M33" t="n">
-        <v>17.185</v>
-      </c>
-      <c r="N33" t="n">
-        <v>29.207</v>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -4906,169 +4912,346 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Lithuania</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-5428.807777775573</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.735666666666</v>
+      </c>
+      <c r="F34" t="n">
+        <v>36880335.97316612</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-37012.58894130614</v>
+      </c>
+      <c r="H34" t="n">
+        <v>9.286333318611</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L34" t="n">
+        <v>23.735666666667</v>
+      </c>
+      <c r="M34" t="n">
+        <v>17.185</v>
+      </c>
+      <c r="N34" t="n">
+        <v>29.207</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>Estonia</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>(0.0, 0.0)</t>
         </is>
       </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
         <v>20734.14195285581</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E35" t="n">
         <v>-10.373068571428</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F35" t="n">
         <v>-7001906.072465623</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G35" t="n">
         <v>7024.583458417419</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H35" t="n">
         <v>-1.761822320809</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N34" t="n">
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
         <v>25.666666666667</v>
       </c>
-      <c r="O34" t="n">
+      <c r="O35" t="n">
         <v>73.59705</v>
       </c>
-      <c r="P34" t="n">
+      <c r="P35" t="n">
         <v>38.26625</v>
       </c>
-      <c r="Q34" t="n">
+      <c r="Q35" t="n">
         <v>3.333333333333</v>
       </c>
-      <c r="R34" t="n">
+      <c r="R35" t="n">
         <v>2</v>
       </c>
-      <c r="S34" t="n">
+      <c r="S35" t="n">
         <v>3</v>
       </c>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AF34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AG34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AH34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AI34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AK34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AL34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AM34" t="inlineStr">
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM35" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5085,7 +5268,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM34"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9386,7 +9569,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -9398,19 +9581,19 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>-99147.19999998058</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>49.79999999999</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>52331890.71687575</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>-52565.39991660103</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>13.199999979081</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -9425,14 +9608,20 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L33" t="n">
-        <v>58.8</v>
-      </c>
-      <c r="M33" t="n">
-        <v>95.40000000000001</v>
-      </c>
-      <c r="N33" t="n">
-        <v>158.4</v>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -9563,169 +9752,346 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Lithuania</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-99147.19999998058</v>
+      </c>
+      <c r="E34" t="n">
+        <v>49.79999999999</v>
+      </c>
+      <c r="F34" t="n">
+        <v>52331890.71687575</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-52565.39991660103</v>
+      </c>
+      <c r="H34" t="n">
+        <v>13.199999979081</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L34" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="M34" t="n">
+        <v>95.40000000000001</v>
+      </c>
+      <c r="N34" t="n">
+        <v>158.4</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>Estonia</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>(0.0, 0.0)</t>
         </is>
       </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
         <v>592.937142856958</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E35" t="n">
         <v>-0.291428571428</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F35" t="n">
         <v>2178662.32332982</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G35" t="n">
         <v>-2182.180714759127</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H35" t="n">
         <v>0.546428571547</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N34" t="n">
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
         <v>10.8</v>
       </c>
-      <c r="O34" t="n">
+      <c r="O35" t="n">
         <v>16.2</v>
       </c>
-      <c r="P34" t="n">
+      <c r="P35" t="n">
         <v>9.6</v>
       </c>
-      <c r="Q34" t="n">
+      <c r="Q35" t="n">
         <v>8.4</v>
       </c>
-      <c r="R34" t="n">
+      <c r="R35" t="n">
         <v>7.2</v>
       </c>
-      <c r="S34" t="n">
+      <c r="S35" t="n">
         <v>14.4</v>
       </c>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AF34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AG34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AH34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AI34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AK34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AL34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AM34" t="inlineStr">
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM35" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9742,7 +10108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM32"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13286,7 +13652,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -13298,113 +13664,167 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>318.094471451535</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.156444422204</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>-154410.2332071213</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>154.242473911737</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.03851689233</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="M28" t="n">
-        <v>4.636363636364</v>
-      </c>
-      <c r="N28" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="O28" t="n">
-        <v>3.558823529412</v>
-      </c>
-      <c r="P28" t="n">
-        <v>5.761904761905</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>5.761904761905</v>
-      </c>
-      <c r="R28" t="n">
-        <v>7.670476190476</v>
-      </c>
-      <c r="S28" t="n">
-        <v>14.642857142857</v>
-      </c>
-      <c r="T28" t="n">
-        <v>10.588235294118</v>
-      </c>
-      <c r="U28" t="n">
-        <v>7.866666666667</v>
-      </c>
-      <c r="V28" t="n">
-        <v>7.263157894737</v>
-      </c>
-      <c r="W28" t="n">
-        <v>5.777777777778</v>
-      </c>
-      <c r="X28" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>5.41567</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>7.517215</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>5.468815</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>8.191847826087001</v>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="AD28" t="n">
-        <v>3.783742424242</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>0.841179487179</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>0.941625</v>
-      </c>
-      <c r="AG28" t="n">
-        <v>0.592875</v>
-      </c>
-      <c r="AH28" t="n">
-        <v>0.592875</v>
-      </c>
-      <c r="AI28" t="n">
-        <v>0.4743</v>
-      </c>
-      <c r="AJ28" t="n">
-        <v>1.070062580645</v>
-      </c>
-      <c r="AK28" t="n">
-        <v>1.19654</v>
-      </c>
-      <c r="AL28" t="n">
-        <v>1.445906666667</v>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AM28" t="inlineStr">
         <is>
@@ -13415,7 +13835,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -13427,103 +13847,81 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-741.764204484433</v>
+        <v>318.094471451535</v>
       </c>
       <c r="E29" t="n">
-        <v>0.371006100729</v>
+        <v>-0.156444422204</v>
       </c>
       <c r="F29" t="n">
-        <v>-143314.1684743426</v>
+        <v>-154410.2332071213</v>
       </c>
       <c r="G29" t="n">
-        <v>142.349311737595</v>
+        <v>154.242473911737</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.035346310777</v>
+        <v>-0.03851689233</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="M29" t="n">
+        <v>4.636363636364</v>
+      </c>
+      <c r="N29" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="O29" t="n">
+        <v>3.558823529412</v>
+      </c>
+      <c r="P29" t="n">
+        <v>5.761904761905</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>5.761904761905</v>
+      </c>
+      <c r="R29" t="n">
+        <v>7.670476190476</v>
       </c>
       <c r="S29" t="n">
-        <v>0</v>
+        <v>14.642857142857</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>10.588235294118</v>
       </c>
       <c r="U29" t="n">
-        <v>0</v>
+        <v>7.866666666667</v>
       </c>
       <c r="V29" t="n">
-        <v>0</v>
+        <v>7.263157894737</v>
       </c>
       <c r="W29" t="n">
-        <v>0</v>
+        <v>5.777777777778</v>
       </c>
       <c r="X29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y29" t="n">
-        <v>4.244541484716</v>
-      </c>
-      <c r="Z29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>5.41567</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>7.517215</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>5.468815</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>8.191847826087001</v>
       </c>
       <c r="AC29" t="inlineStr">
         <is>
@@ -13531,31 +13929,31 @@
         </is>
       </c>
       <c r="AD29" t="n">
-        <v>4.080878285714</v>
+        <v>3.783742424242</v>
       </c>
       <c r="AE29" t="n">
-        <v>6.073748232984</v>
+        <v>0.841179487179</v>
       </c>
       <c r="AF29" t="n">
-        <v>9.604757646154001</v>
+        <v>0.941625</v>
       </c>
       <c r="AG29" t="n">
-        <v>7.405418547672</v>
+        <v>0.592875</v>
       </c>
       <c r="AH29" t="n">
-        <v>4.450726694045</v>
+        <v>0.592875</v>
       </c>
       <c r="AI29" t="n">
-        <v>5.642628833992</v>
+        <v>0.4743</v>
       </c>
       <c r="AJ29" t="n">
-        <v>4.670536099624</v>
+        <v>1.070062580645</v>
       </c>
       <c r="AK29" t="n">
-        <v>5.077649344485</v>
+        <v>1.19654</v>
       </c>
       <c r="AL29" t="n">
-        <v>4.657920520646</v>
+        <v>1.445906666667</v>
       </c>
       <c r="AM29" t="inlineStr">
         <is>
@@ -13566,7 +13964,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -13685,40 +14083,60 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AB30" t="n">
-        <v>0</v>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC30" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="AD30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL30" t="n">
-        <v>0</v>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AM30" t="inlineStr">
         <is>
@@ -13729,7 +14147,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -13741,79 +14159,103 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>4114.612607193243</v>
+        <v>-741.764204484433</v>
       </c>
       <c r="E31" t="n">
-        <v>-2.042350397733</v>
+        <v>0.371006100729</v>
       </c>
       <c r="F31" t="n">
-        <v>512393.0377879965</v>
+        <v>-143314.1684743426</v>
       </c>
       <c r="G31" t="n">
-        <v>-509.30057873856</v>
+        <v>142.349311737595</v>
       </c>
       <c r="H31" t="n">
-        <v>0.126557762555</v>
+        <v>-0.035346310777</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
-      <c r="J31" t="n">
-        <v>53.886048083598</v>
-      </c>
-      <c r="K31" t="n">
-        <v>64.800423952033</v>
-      </c>
-      <c r="L31" t="n">
-        <v>62.93524</v>
-      </c>
-      <c r="M31" t="n">
-        <v>36.231787096774</v>
-      </c>
-      <c r="N31" t="n">
-        <v>57.585765217391</v>
-      </c>
-      <c r="O31" t="n">
-        <v>43.606662068966</v>
-      </c>
-      <c r="P31" t="n">
-        <v>39.916259677419</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>43.308605172414</v>
-      </c>
-      <c r="R31" t="n">
-        <v>35.155967567568</v>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S31" t="n">
-        <v>22.890024274155</v>
+        <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>21.59842845881</v>
+        <v>0</v>
       </c>
       <c r="U31" t="n">
-        <v>22.51419778002</v>
+        <v>0</v>
       </c>
       <c r="V31" t="n">
-        <v>13.282339395717</v>
+        <v>0</v>
       </c>
       <c r="W31" t="n">
-        <v>11.091394018205</v>
+        <v>0</v>
       </c>
       <c r="X31" t="n">
-        <v>6.247894183602</v>
+        <v>0</v>
       </c>
       <c r="Y31" t="n">
-        <v>6.367228111088</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>5.789944692412</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>5.555056360709</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>5.011841890791</v>
+        <v>4.244541484716</v>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC31" t="inlineStr">
         <is>
@@ -13821,31 +14263,31 @@
         </is>
       </c>
       <c r="AD31" t="n">
-        <v>10.173906987542</v>
+        <v>4.080878285714</v>
       </c>
       <c r="AE31" t="n">
-        <v>7.433573984155</v>
+        <v>6.073748232984</v>
       </c>
       <c r="AF31" t="n">
-        <v>6.935008474576</v>
+        <v>9.604757646154001</v>
       </c>
       <c r="AG31" t="n">
-        <v>6.93986100951</v>
+        <v>7.405418547672</v>
       </c>
       <c r="AH31" t="n">
-        <v>4.752558772936</v>
+        <v>4.450726694045</v>
       </c>
       <c r="AI31" t="n">
-        <v>3.719779370433</v>
+        <v>5.642628833992</v>
       </c>
       <c r="AJ31" t="n">
-        <v>5.444959962317</v>
+        <v>4.670536099624</v>
       </c>
       <c r="AK31" t="n">
-        <v>6.257965223881</v>
+        <v>5.077649344485</v>
       </c>
       <c r="AL31" t="n">
-        <v>9.566514039566</v>
+        <v>4.657920520646</v>
       </c>
       <c r="AM31" t="inlineStr">
         <is>
@@ -13856,125 +14298,598 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>Bosnia and Herzegovina</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Iceland</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Lithuania</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4114.612607193243</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-2.042350397733</v>
+      </c>
+      <c r="F34" t="n">
+        <v>512393.0377879965</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-509.30057873856</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.126557762555</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>53.886048083598</v>
+      </c>
+      <c r="K34" t="n">
+        <v>64.800423952033</v>
+      </c>
+      <c r="L34" t="n">
+        <v>62.93524</v>
+      </c>
+      <c r="M34" t="n">
+        <v>36.231787096774</v>
+      </c>
+      <c r="N34" t="n">
+        <v>57.585765217391</v>
+      </c>
+      <c r="O34" t="n">
+        <v>43.606662068966</v>
+      </c>
+      <c r="P34" t="n">
+        <v>39.916259677419</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>43.308605172414</v>
+      </c>
+      <c r="R34" t="n">
+        <v>35.155967567568</v>
+      </c>
+      <c r="S34" t="n">
+        <v>22.890024274155</v>
+      </c>
+      <c r="T34" t="n">
+        <v>21.59842845881</v>
+      </c>
+      <c r="U34" t="n">
+        <v>22.51419778002</v>
+      </c>
+      <c r="V34" t="n">
+        <v>13.282339395717</v>
+      </c>
+      <c r="W34" t="n">
+        <v>11.091394018205</v>
+      </c>
+      <c r="X34" t="n">
+        <v>6.247894183602</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>6.367228111088</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>5.789944692412</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>5.555056360709</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>5.011841890791</v>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD34" t="n">
+        <v>10.173906987542</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>7.433573984155</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>6.935008474576</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>6.93986100951</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>4.752558772936</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>3.719779370433</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>5.444959962317</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>6.257965223881</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>9.566514039566</v>
+      </c>
+      <c r="AM34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>Estonia</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>(0.0, 0.0)</t>
         </is>
       </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="n">
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
         <v>1174.185759398031</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E35" t="n">
         <v>-0.5753745364940001</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F35" t="n">
         <v>21637.298442837</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G35" t="n">
         <v>-20.997414449849</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H35" t="n">
         <v>0.00509517152</v>
       </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="n">
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
         <v>22.797902687068</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K35" t="n">
         <v>23.31694531506</v>
       </c>
-      <c r="L32" t="n">
+      <c r="L35" t="n">
         <v>27.612428571429</v>
       </c>
-      <c r="M32" t="n">
+      <c r="M35" t="n">
         <v>27.863357142857</v>
       </c>
-      <c r="N32" t="n">
+      <c r="N35" t="n">
         <v>22.535357142857</v>
       </c>
-      <c r="O32" t="n">
+      <c r="O35" t="n">
         <v>9.134928571429</v>
       </c>
-      <c r="P32" t="n">
+      <c r="P35" t="n">
         <v>56.555075471698</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="Q35" t="n">
         <v>42.461185185185</v>
       </c>
-      <c r="R32" t="n">
+      <c r="R35" t="n">
         <v>33.534976744186</v>
       </c>
-      <c r="S32" t="n">
+      <c r="S35" t="n">
         <v>21.411975337918</v>
       </c>
-      <c r="T32" t="n">
+      <c r="T35" t="n">
         <v>26.860010955302</v>
       </c>
-      <c r="U32" t="n">
+      <c r="U35" t="n">
         <v>23.768869883934</v>
       </c>
-      <c r="V32" t="n">
+      <c r="V35" t="n">
         <v>22.619252567516</v>
       </c>
-      <c r="W32" t="n">
+      <c r="W35" t="n">
         <v>19.901978590544</v>
       </c>
-      <c r="X32" t="n">
+      <c r="X35" t="n">
         <v>13.553119959677</v>
       </c>
-      <c r="Y32" t="n">
+      <c r="Y35" t="n">
         <v>11.324840450865</v>
       </c>
-      <c r="Z32" t="n">
+      <c r="Z35" t="n">
         <v>12.326844718628</v>
       </c>
-      <c r="AA32" t="n">
+      <c r="AA35" t="n">
         <v>13.355444015444</v>
       </c>
-      <c r="AB32" t="n">
+      <c r="AB35" t="n">
         <v>14.245692555214</v>
       </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD32" t="n">
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD35" t="n">
         <v>19.397555173781</v>
       </c>
-      <c r="AE32" t="n">
+      <c r="AE35" t="n">
         <v>18.43027027027</v>
       </c>
-      <c r="AF32" t="n">
+      <c r="AF35" t="n">
         <v>16.229675108723</v>
       </c>
-      <c r="AG32" t="n">
+      <c r="AG35" t="n">
         <v>16.43513143483</v>
       </c>
-      <c r="AH32" t="n">
+      <c r="AH35" t="n">
         <v>14.950217273221</v>
       </c>
-      <c r="AI32" t="n">
+      <c r="AI35" t="n">
         <v>15.991583166333</v>
       </c>
-      <c r="AJ32" t="n">
+      <c r="AJ35" t="n">
         <v>14.364621621622</v>
       </c>
-      <c r="AK32" t="n">
+      <c r="AK35" t="n">
         <v>15.295330335028</v>
       </c>
-      <c r="AL32" t="n">
+      <c r="AL35" t="n">
         <v>18.387573849563</v>
       </c>
-      <c r="AM32" t="inlineStr">
+      <c r="AM35" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -13991,7 +14906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM32"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17535,7 +18450,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -17547,113 +18462,167 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>313.490745014007</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.155068934314</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>17545.66208528776</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>-17.350553790911</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>0.004289645588</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
-      <c r="J28" t="n">
-        <v>3.561744966443</v>
-      </c>
-      <c r="K28" t="n">
-        <v>5.129343065693</v>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="M28" t="n">
-        <v>6.218181818182</v>
-      </c>
-      <c r="N28" t="n">
-        <v>6.75</v>
-      </c>
-      <c r="O28" t="n">
-        <v>4.341176470588</v>
-      </c>
-      <c r="P28" t="n">
-        <v>3.771428571429</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>2.228571428571</v>
-      </c>
-      <c r="R28" t="n">
-        <v>3.085714285714</v>
-      </c>
-      <c r="S28" t="n">
-        <v>3.342857142857</v>
-      </c>
-      <c r="T28" t="n">
-        <v>3.811764705882</v>
-      </c>
-      <c r="U28" t="n">
-        <v>3.12</v>
-      </c>
-      <c r="V28" t="n">
-        <v>2.463157894737</v>
-      </c>
-      <c r="W28" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="X28" t="n">
-        <v>2.475</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>2.34</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>2.191304347826</v>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="AD28" t="n">
-        <v>1.745454545455</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>0.738461538462</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="AG28" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="AH28" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="AI28" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="AJ28" t="n">
-        <v>1.202161290323</v>
-      </c>
-      <c r="AK28" t="n">
-        <v>1.206121212121</v>
-      </c>
-      <c r="AL28" t="n">
-        <v>1.722291666667</v>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AM28" t="inlineStr">
         <is>
@@ -17664,7 +18633,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -17676,103 +18645,81 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-404.182728191494</v>
+        <v>313.490745014007</v>
       </c>
       <c r="E29" t="n">
-        <v>0.202181663791</v>
+        <v>-0.155068934314</v>
       </c>
       <c r="F29" t="n">
-        <v>-56721.46736898353</v>
+        <v>17545.66208528776</v>
       </c>
       <c r="G29" t="n">
-        <v>56.284792406851</v>
+        <v>-17.350553790911</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.013962086529</v>
+        <v>0.004289645588</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J29" t="n">
+        <v>3.561744966443</v>
+      </c>
+      <c r="K29" t="n">
+        <v>5.129343065693</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="M29" t="n">
+        <v>6.218181818182</v>
+      </c>
+      <c r="N29" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="O29" t="n">
+        <v>4.341176470588</v>
+      </c>
+      <c r="P29" t="n">
+        <v>3.771428571429</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>2.228571428571</v>
+      </c>
+      <c r="R29" t="n">
+        <v>3.085714285714</v>
       </c>
       <c r="S29" t="n">
-        <v>0</v>
+        <v>3.342857142857</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>3.811764705882</v>
       </c>
       <c r="U29" t="n">
-        <v>0</v>
+        <v>3.12</v>
       </c>
       <c r="V29" t="n">
-        <v>0</v>
+        <v>2.463157894737</v>
       </c>
       <c r="W29" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="X29" t="n">
-        <v>2.015094339623</v>
+        <v>2.475</v>
       </c>
       <c r="Y29" t="n">
-        <v>1.30480349345</v>
-      </c>
-      <c r="Z29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>2.34</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>2.191304347826</v>
       </c>
       <c r="AC29" t="inlineStr">
         <is>
@@ -17780,31 +18727,31 @@
         </is>
       </c>
       <c r="AD29" t="n">
-        <v>2.01974025974</v>
+        <v>1.745454545455</v>
       </c>
       <c r="AE29" t="n">
-        <v>2.337172774869</v>
+        <v>0.738461538462</v>
       </c>
       <c r="AF29" t="n">
-        <v>5.383384615385</v>
+        <v>1.05</v>
       </c>
       <c r="AG29" t="n">
-        <v>3.272727272727</v>
+        <v>1.05</v>
       </c>
       <c r="AH29" t="n">
-        <v>3.082546201232</v>
+        <v>1.35</v>
       </c>
       <c r="AI29" t="n">
-        <v>2.554150197628</v>
+        <v>1.08</v>
       </c>
       <c r="AJ29" t="n">
-        <v>3.248120300752</v>
+        <v>1.202161290323</v>
       </c>
       <c r="AK29" t="n">
-        <v>3.280256781193</v>
+        <v>1.206121212121</v>
       </c>
       <c r="AL29" t="n">
-        <v>2.697026929982</v>
+        <v>1.722291666667</v>
       </c>
       <c r="AM29" t="inlineStr">
         <is>
@@ -17815,7 +18762,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -17827,19 +18774,19 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>28386.28701261156</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>-14.073642229343</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>12605822.30612083</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>-12509.42622539343</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>3.103444084663</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -17934,40 +18881,60 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AB30" t="n">
-        <v>204</v>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC30" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="AD30" t="n">
-        <v>68</v>
-      </c>
-      <c r="AE30" t="n">
-        <v>54</v>
-      </c>
-      <c r="AF30" t="n">
-        <v>40.8</v>
-      </c>
-      <c r="AG30" t="n">
-        <v>34</v>
-      </c>
-      <c r="AH30" t="n">
-        <v>27.428571428571</v>
-      </c>
-      <c r="AI30" t="n">
-        <v>24</v>
-      </c>
-      <c r="AJ30" t="n">
-        <v>21.333333333333</v>
-      </c>
-      <c r="AK30" t="n">
-        <v>18.348</v>
-      </c>
-      <c r="AL30" t="n">
-        <v>12.247575757576</v>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AM30" t="inlineStr">
         <is>
@@ -17978,7 +18945,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -17990,79 +18957,103 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>527.6992428980139</v>
+        <v>-404.182728191494</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.260150468728</v>
+        <v>0.202181663791</v>
       </c>
       <c r="F31" t="n">
-        <v>24408.01730140436</v>
+        <v>-56721.46736898353</v>
       </c>
       <c r="G31" t="n">
-        <v>-24.092536874396</v>
+        <v>56.284792406851</v>
       </c>
       <c r="H31" t="n">
-        <v>0.005946031688</v>
+        <v>-0.013962086529</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
-      <c r="J31" t="n">
-        <v>6.216197051689</v>
-      </c>
-      <c r="K31" t="n">
-        <v>6.484204379562</v>
-      </c>
-      <c r="L31" t="n">
-        <v>7.704</v>
-      </c>
-      <c r="M31" t="n">
-        <v>10.451612903226</v>
-      </c>
-      <c r="N31" t="n">
-        <v>11.895652173913</v>
-      </c>
-      <c r="O31" t="n">
-        <v>12.786206896552</v>
-      </c>
-      <c r="P31" t="n">
-        <v>11.264516129032</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>14.648275862069</v>
-      </c>
-      <c r="R31" t="n">
-        <v>10.994594594595</v>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S31" t="n">
-        <v>7.941932413137</v>
+        <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>7.918013401655</v>
+        <v>0</v>
       </c>
       <c r="U31" t="n">
-        <v>7.356205852674</v>
+        <v>0</v>
       </c>
       <c r="V31" t="n">
-        <v>4.704605456145</v>
+        <v>0</v>
       </c>
       <c r="W31" t="n">
-        <v>3.623407022107</v>
+        <v>0</v>
       </c>
       <c r="X31" t="n">
-        <v>3.2543798178</v>
+        <v>2.015094339623</v>
       </c>
       <c r="Y31" t="n">
-        <v>3.125291498834</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>3.049485736464</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>3.101449275362</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>2.904645476773</v>
+        <v>1.30480349345</v>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC31" t="inlineStr">
         <is>
@@ -18070,31 +19061,31 @@
         </is>
       </c>
       <c r="AD31" t="n">
-        <v>6.602182155846</v>
+        <v>2.01974025974</v>
       </c>
       <c r="AE31" t="n">
-        <v>3.703041144902</v>
+        <v>2.337172774869</v>
       </c>
       <c r="AF31" t="n">
-        <v>3.874576271186</v>
+        <v>5.383384615385</v>
       </c>
       <c r="AG31" t="n">
-        <v>3.950256035113</v>
+        <v>3.272727272727</v>
       </c>
       <c r="AH31" t="n">
-        <v>4.025229357798</v>
+        <v>3.082546201232</v>
       </c>
       <c r="AI31" t="n">
-        <v>4.097807757167</v>
+        <v>2.554150197628</v>
       </c>
       <c r="AJ31" t="n">
-        <v>4.437117286858</v>
+        <v>3.248120300752</v>
       </c>
       <c r="AK31" t="n">
-        <v>5.142089552239</v>
+        <v>3.280256781193</v>
       </c>
       <c r="AL31" t="n">
-        <v>4.059476707084</v>
+        <v>2.697026929982</v>
       </c>
       <c r="AM31" t="inlineStr">
         <is>
@@ -18105,125 +19096,598 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>Bosnia and Herzegovina</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Iceland</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>28386.28701261156</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-14.073642229343</v>
+      </c>
+      <c r="F33" t="n">
+        <v>12605822.30612083</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-12509.42622539343</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3.103444084663</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB33" t="n">
+        <v>204</v>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD33" t="n">
+        <v>68</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>54</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>34</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>27.428571428571</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>24</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>21.333333333333</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>18.348</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>12.247575757576</v>
+      </c>
+      <c r="AM33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Lithuania</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>527.6992428980139</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-0.260150468728</v>
+      </c>
+      <c r="F34" t="n">
+        <v>24408.01730140436</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-24.092536874396</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.005946031688</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>6.216197051689</v>
+      </c>
+      <c r="K34" t="n">
+        <v>6.484204379562</v>
+      </c>
+      <c r="L34" t="n">
+        <v>7.704</v>
+      </c>
+      <c r="M34" t="n">
+        <v>10.451612903226</v>
+      </c>
+      <c r="N34" t="n">
+        <v>11.895652173913</v>
+      </c>
+      <c r="O34" t="n">
+        <v>12.786206896552</v>
+      </c>
+      <c r="P34" t="n">
+        <v>11.264516129032</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>14.648275862069</v>
+      </c>
+      <c r="R34" t="n">
+        <v>10.994594594595</v>
+      </c>
+      <c r="S34" t="n">
+        <v>7.941932413137</v>
+      </c>
+      <c r="T34" t="n">
+        <v>7.918013401655</v>
+      </c>
+      <c r="U34" t="n">
+        <v>7.356205852674</v>
+      </c>
+      <c r="V34" t="n">
+        <v>4.704605456145</v>
+      </c>
+      <c r="W34" t="n">
+        <v>3.623407022107</v>
+      </c>
+      <c r="X34" t="n">
+        <v>3.2543798178</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>3.125291498834</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>3.049485736464</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>3.101449275362</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>2.904645476773</v>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD34" t="n">
+        <v>6.602182155846</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>3.703041144902</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>3.874576271186</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>3.950256035113</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>4.025229357798</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>4.097807757167</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>4.437117286858</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>5.142089552239</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>4.059476707084</v>
+      </c>
+      <c r="AM34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>Estonia</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>(0.0, 0.0)</t>
         </is>
       </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="n">
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
         <v>-1369.39571244151</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E35" t="n">
         <v>0.688978852027</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F35" t="n">
         <v>90828.92174011859</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G35" t="n">
         <v>-91.324281695781</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H35" t="n">
         <v>0.022956734321</v>
       </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="n">
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
         <v>7.005555407459</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K35" t="n">
         <v>7.664153135707</v>
       </c>
-      <c r="L32" t="n">
+      <c r="L35" t="n">
         <v>8.4</v>
       </c>
-      <c r="M32" t="n">
+      <c r="M35" t="n">
         <v>0.771428571429</v>
       </c>
-      <c r="N32" t="n">
+      <c r="N35" t="n">
         <v>1.457142857143</v>
       </c>
-      <c r="O32" t="n">
+      <c r="O35" t="n">
         <v>2.314285714286</v>
       </c>
-      <c r="P32" t="n">
+      <c r="P35" t="n">
         <v>3.939622641509</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="Q35" t="n">
         <v>5.666666666667</v>
       </c>
-      <c r="R32" t="n">
+      <c r="R35" t="n">
         <v>8.037209302326</v>
       </c>
-      <c r="S32" t="n">
+      <c r="S35" t="n">
         <v>7.452691486839</v>
       </c>
-      <c r="T32" t="n">
+      <c r="T35" t="n">
         <v>7.382997370727</v>
       </c>
-      <c r="U32" t="n">
+      <c r="U35" t="n">
         <v>7.191203420892</v>
       </c>
-      <c r="V32" t="n">
+      <c r="V35" t="n">
         <v>8.010650437429</v>
       </c>
-      <c r="W32" t="n">
+      <c r="W35" t="n">
         <v>7.341302408564</v>
       </c>
-      <c r="X32" t="n">
+      <c r="X35" t="n">
         <v>7.403225806452</v>
       </c>
-      <c r="Y32" t="n">
+      <c r="Y35" t="n">
         <v>7.201143038578</v>
       </c>
-      <c r="Z32" t="n">
+      <c r="Z35" t="n">
         <v>13.016551309058</v>
       </c>
-      <c r="AA32" t="n">
+      <c r="AA35" t="n">
         <v>15.984555984556</v>
       </c>
-      <c r="AB32" t="n">
+      <c r="AB35" t="n">
         <v>17.63931548925</v>
       </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD32" t="n">
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD35" t="n">
         <v>16.698823840359</v>
       </c>
-      <c r="AE32" t="n">
+      <c r="AE35" t="n">
         <v>16.394594594595</v>
       </c>
-      <c r="AF32" t="n">
+      <c r="AF35" t="n">
         <v>16.761320030698</v>
       </c>
-      <c r="AG32" t="n">
+      <c r="AG35" t="n">
         <v>17.49726177437</v>
       </c>
-      <c r="AH32" t="n">
+      <c r="AH35" t="n">
         <v>17.94133623031</v>
       </c>
-      <c r="AI32" t="n">
+      <c r="AI35" t="n">
         <v>19.01517320355</v>
       </c>
-      <c r="AJ32" t="n">
+      <c r="AJ35" t="n">
         <v>19.605405405405</v>
       </c>
-      <c r="AK32" t="n">
+      <c r="AK35" t="n">
         <v>23.042628079781</v>
       </c>
-      <c r="AL32" t="n">
+      <c r="AL35" t="n">
         <v>22.620258114978</v>
       </c>
-      <c r="AM32" t="inlineStr">
+      <c r="AM35" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>